<commit_message>
update to new orders
</commit_message>
<xml_diff>
--- a/run-orders/xlsx/peep-run-orders.xlsx
+++ b/run-orders/xlsx/peep-run-orders.xlsx
@@ -98,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,6 +110,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -251,8 +267,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -398,7 +416,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,7 +751,7 @@
   <dimension ref="A1:BN3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1351,7 +1371,7 @@
   <dimension ref="A1:BN3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B42" activeCellId="1" sqref="A1:A1048576 B42"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3221,19 +3241,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
+      <c r="D1" s="21" t="s">
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>3</v>
+      <c r="F1" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
@@ -3269,7 +3289,7 @@
         <v>2</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>2</v>
@@ -3413,7 +3433,7 @@
         <v>2</v>
       </c>
       <c r="BN1" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:66">
@@ -3426,14 +3446,14 @@
       <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="26" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>7</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>6</v>
@@ -3621,19 +3641,19 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4">
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -3669,7 +3689,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S3" s="4">
         <v>0</v>
@@ -3813,7 +3833,7 @@
         <v>0</v>
       </c>
       <c r="BN3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3831,7 +3851,7 @@
   <dimension ref="A1:BN3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5081,7 +5101,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -5111,7 +5131,7 @@
         <v>2</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>2</v>
@@ -5273,7 +5293,7 @@
         <v>2</v>
       </c>
       <c r="BN1" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:66">
@@ -5481,7 +5501,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3" s="4">
         <v>0</v>
@@ -5511,7 +5531,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M3" s="4">
         <v>0</v>
@@ -5673,7 +5693,7 @@
         <v>0</v>
       </c>
       <c r="BN3" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>